<commit_message>
Hieu chinh ke hoach report
</commit_message>
<xml_diff>
--- a/02 Checklist training/TOOL.xlsx
+++ b/02 Checklist training/TOOL.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_AAFD4EFB2B63699904F41A0064FC4A6366F7D554" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36CA8300-D8F6-4D00-997E-DF9436C25E39}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB27C00-627F-4F8D-8423-D38183F5492F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GHS" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="DOOR" sheetId="3" r:id="rId5"/>
     <sheet name="EBtresos" sheetId="4" r:id="rId6"/>
     <sheet name="Perl" sheetId="7" r:id="rId7"/>
+    <sheet name="Report_thuc hien" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>ARM</t>
   </si>
@@ -395,12 +396,15 @@
   <si>
     <t>Vào edit enviroment variable</t>
   </si>
+  <si>
+    <t>Noi dung cac file nay van con mot so muc chua thuc hien xong</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,7 +515,7 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>114300</xdr:colOff>
           <xdr:row>41</xdr:row>
-          <xdr:rowOff>155575</xdr:rowOff>
+          <xdr:rowOff>158750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1197,16 +1201,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="19" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="19.5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1222,62 +1226,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="19.5">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
       <c r="J21" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
       <c r="J22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.4">
       <c r="J24" s="1" t="s">
         <v>15</v>
       </c>
@@ -1308,7 +1312,7 @@
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>114300</xdr:colOff>
                 <xdr:row>41</xdr:row>
-                <xdr:rowOff>155575</xdr:rowOff>
+                <xdr:rowOff>158750</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1330,22 +1334,22 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="19" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="3:6">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="3:6">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1353,17 +1357,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="3:6">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="3:6">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="3:6">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1385,102 +1389,102 @@
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="19" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C20" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B48" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C49" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="3:4">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C50" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="3:4">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.4">
       <c r="D51" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="3:4">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C52" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="3:4">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.4">
       <c r="D53" s="1" t="s">
         <v>41</v>
       </c>
@@ -1499,17 +1503,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="19" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="3:3">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1530,42 +1534,42 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="19" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="3:12">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="3:12">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.4">
       <c r="L6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="3:12">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.4">
       <c r="L8" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C59" s="1" t="s">
         <v>50</v>
       </c>
@@ -1580,117 +1584,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="19" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="3:5">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C6" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.4">
       <c r="D7" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.4">
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.4">
       <c r="E9" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="3:5" ht="19.5">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C13" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="3:5">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C15" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C17" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C18" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C20" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C21" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C23" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B27" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C28" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C29" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="19.5"/>
-    <row r="32" spans="2:3" ht="19.5">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C32" s="1" t="s">
         <v>69</v>
       </c>
@@ -1710,36 +1713,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="19" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
       <c r="L24" s="1" t="s">
         <v>74</v>
       </c>
@@ -1747,6 +1750,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D89879B-095F-4B84-97DC-9C0F9EEFCF72}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1762,15 +1785,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E27BAF8570EFEB4EB503BF1DEDEAC3FF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f040904d2061e92c1c49887913d46edd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8f1bc372-0378-4844-8faa-948093c5494b" xmlns:ns3="98414995-779f-42fe-85cc-b2ed736cde9d" xmlns:ns4="c4672b8b-43e2-4139-8cd1-27ad03f081e7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09ab51ae3e7defa84a5119748a6783d4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="8f1bc372-0378-4844-8faa-948093c5494b"/>
@@ -2006,14 +2020,50 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B62A3E1B-B304-4BD7-9F01-5171084042AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B62A3E1B-B304-4BD7-9F01-5171084042AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
+    <ds:schemaRef ds:uri="8f1bc372-0378-4844-8faa-948093c5494b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B998FA5-8041-4895-99F2-9F0FF90E80B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2C0E2D0-9FE6-4FE1-AB8A-94FAE1E8D669}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8f1bc372-0378-4844-8faa-948093c5494b"/>
+    <ds:schemaRef ds:uri="98414995-779f-42fe-85cc-b2ed736cde9d"/>
+    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2C0E2D0-9FE6-4FE1-AB8A-94FAE1E8D669}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B998FA5-8041-4895-99F2-9F0FF90E80B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>